<commit_message>
add M45 and M102
</commit_message>
<xml_diff>
--- a/SmartHandController/Catalog.xlsx
+++ b/SmartHandController/Catalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\GitHub\TeenAstro\SmartHandController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60D451A6-F7F1-499F-9C80-479F7FE3FBE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE276AA-FC81-4AF5-828F-B6EE1D235975}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="1725" windowWidth="18000" windowHeight="9360" activeTab="2" xr2:uid="{983D245A-AE43-4906-82C2-4606C1D254C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{983D245A-AE43-4906-82C2-4606C1D254C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Messier" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{942127E5-A596-4E77-AF44-2F423C350B23}">
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="G1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,15 +442,15 @@
         <v>-0.82330000000000003</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G65" si="0">RIGHT("              "&amp;TRUNC((D2+200)/10),4)</f>
+        <f t="shared" ref="G2:G66" si="0">RIGHT("              "&amp;TRUNC((D2+200)/10),4)</f>
         <v xml:space="preserve">  82</v>
       </c>
       <c r="H2" s="2" t="str">
-        <f t="shared" ref="H2:H65" si="1">RIGHT("              " &amp;TRUNC(E2*65536 / 24),6)</f>
+        <f t="shared" ref="H2:H66" si="1">RIGHT("              " &amp;TRUNC(E2*65536 / 24),6)</f>
         <v xml:space="preserve"> 58866</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f t="shared" ref="I2:I65" si="2">RIGHT("              " &amp; TRUNC(F2*32767 / 90),6)</f>
+        <f t="shared" ref="I2:I66" si="2">RIGHT("              " &amp; TRUNC(F2*32767 / 90),6)</f>
         <v xml:space="preserve">  -299</v>
       </c>
     </row>
@@ -1771,35 +1767,32 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>67</v>
-      </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D44">
-        <v>610</v>
+        <v>160</v>
       </c>
       <c r="E44">
-        <v>7.6962999999999999</v>
+        <v>3.783083</v>
       </c>
       <c r="F44">
-        <v>-14.81</v>
+        <v>24.1144</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  81</v>
+        <v xml:space="preserve">  36</v>
       </c>
       <c r="H44" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 21016</v>
+        <v xml:space="preserve"> 10330</v>
       </c>
       <c r="I44" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> -5391</v>
+        <v xml:space="preserve">  8779</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -1810,240 +1803,240 @@
         <v>1</v>
       </c>
       <c r="C45">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D45">
-        <v>440</v>
+        <v>610</v>
       </c>
       <c r="E45">
-        <v>7.6097000000000001</v>
+        <v>7.6962999999999999</v>
       </c>
       <c r="F45">
-        <v>-14.4826</v>
+        <v>-14.81</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  64</v>
+        <v xml:space="preserve">  81</v>
       </c>
       <c r="H45" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 20779</v>
+        <v xml:space="preserve"> 21016</v>
       </c>
       <c r="I45" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> -5272</v>
+        <v xml:space="preserve"> -5391</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D46">
-        <v>580</v>
+        <v>440</v>
       </c>
       <c r="E46">
-        <v>8.2286999999999999</v>
+        <v>7.6097000000000001</v>
       </c>
       <c r="F46">
-        <v>-5.7504</v>
+        <v>-14.4826</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  78</v>
+        <v xml:space="preserve">  64</v>
       </c>
       <c r="H46" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 22469</v>
+        <v xml:space="preserve"> 20779</v>
       </c>
       <c r="I46" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> -2093</v>
+        <v xml:space="preserve"> -5272</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D47">
-        <v>1217</v>
+        <v>580</v>
       </c>
       <c r="E47">
-        <v>12.4963</v>
+        <v>8.2286999999999999</v>
       </c>
       <c r="F47">
-        <v>8.0005000000000006</v>
+        <v>-5.7504</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 141</v>
+        <v xml:space="preserve">  78</v>
       </c>
       <c r="H47" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 34123</v>
+        <v xml:space="preserve"> 22469</v>
       </c>
       <c r="I47" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  2912</v>
+        <v xml:space="preserve"> -2093</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D48">
-        <v>590</v>
+        <v>1217</v>
       </c>
       <c r="E48">
-        <v>7.0446</v>
+        <v>12.4963</v>
       </c>
       <c r="F48">
-        <v>-8.3640000000000008</v>
+        <v>8.0005000000000006</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  79</v>
+        <v xml:space="preserve"> 141</v>
       </c>
       <c r="H48" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 19236</v>
+        <v xml:space="preserve"> 34123</v>
       </c>
       <c r="I48" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> -3045</v>
+        <v xml:space="preserve">  2912</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D49">
-        <v>836</v>
+        <v>590</v>
       </c>
       <c r="E49">
-        <v>13.497999999999999</v>
+        <v>7.0446</v>
       </c>
       <c r="F49">
-        <v>47.1952</v>
+        <v>-8.3640000000000008</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 103</v>
+        <v xml:space="preserve">  79</v>
       </c>
       <c r="H49" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 36858</v>
+        <v xml:space="preserve"> 19236</v>
       </c>
       <c r="I49" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> 17182</v>
+        <v xml:space="preserve"> -3045</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D50">
-        <v>690</v>
+        <v>836</v>
       </c>
       <c r="E50">
-        <v>23.413399999999999</v>
+        <v>13.497999999999999</v>
       </c>
       <c r="F50">
-        <v>61.593200000000003</v>
+        <v>47.1952</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  89</v>
+        <v xml:space="preserve"> 103</v>
       </c>
       <c r="H50" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 63934</v>
+        <v xml:space="preserve"> 36858</v>
       </c>
       <c r="I50" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> 22424</v>
+        <v xml:space="preserve"> 17182</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B51">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C51">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D51">
-        <v>779</v>
+        <v>690</v>
       </c>
       <c r="E51">
-        <v>13.215299999999999</v>
+        <v>23.413399999999999</v>
       </c>
       <c r="F51">
-        <v>18.1691</v>
+        <v>61.593200000000003</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  97</v>
+        <v xml:space="preserve">  89</v>
       </c>
       <c r="H51" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 36086</v>
+        <v xml:space="preserve"> 63934</v>
       </c>
       <c r="I51" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  6614</v>
+        <v xml:space="preserve"> 22424</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="B52">
         <v>8</v>
       </c>
       <c r="C52">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D52">
-        <v>770</v>
+        <v>779</v>
       </c>
       <c r="E52">
-        <v>18.9176</v>
+        <v>13.215299999999999</v>
       </c>
       <c r="F52">
-        <v>-30.4785</v>
+        <v>18.1691</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -2051,11 +2044,11 @@
       </c>
       <c r="H52" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 51657</v>
+        <v xml:space="preserve"> 36086</v>
       </c>
       <c r="I52" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>-11096</v>
+        <v xml:space="preserve">  6614</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2066,60 +2059,60 @@
         <v>8</v>
       </c>
       <c r="C53">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D53">
-        <v>649</v>
+        <v>770</v>
       </c>
       <c r="E53">
-        <v>19.666499999999999</v>
+        <v>18.9176</v>
       </c>
       <c r="F53">
-        <v>-30.9621</v>
+        <v>-30.4785</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  84</v>
+        <v xml:space="preserve">  97</v>
       </c>
       <c r="H53" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 53702</v>
+        <v xml:space="preserve"> 51657</v>
       </c>
       <c r="I53" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>-11272</v>
+        <v>-11096</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B54">
         <v>8</v>
       </c>
       <c r="C54">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D54">
-        <v>840</v>
+        <v>649</v>
       </c>
       <c r="E54">
-        <v>19.276499999999999</v>
+        <v>19.666499999999999</v>
       </c>
       <c r="F54">
-        <v>30.1845</v>
+        <v>-30.9621</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 104</v>
+        <v xml:space="preserve">  84</v>
       </c>
       <c r="H54" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 52637</v>
+        <v xml:space="preserve"> 53702</v>
       </c>
       <c r="I54" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> 10989</v>
+        <v>-11272</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2127,63 +2120,63 @@
         <v>51</v>
       </c>
       <c r="B55">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D55">
-        <v>880</v>
+        <v>840</v>
       </c>
       <c r="E55">
-        <v>18.8931</v>
+        <v>19.276499999999999</v>
       </c>
       <c r="F55">
-        <v>33.028599999999997</v>
+        <v>30.1845</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 108</v>
+        <v xml:space="preserve"> 104</v>
       </c>
       <c r="H55" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 51590</v>
+        <v xml:space="preserve"> 52637</v>
       </c>
       <c r="I55" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> 12024</v>
+        <v xml:space="preserve"> 10989</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C56">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D56">
-        <v>966</v>
+        <v>880</v>
       </c>
       <c r="E56">
-        <v>12.6288</v>
+        <v>18.8931</v>
       </c>
       <c r="F56">
-        <v>11.818199999999999</v>
+        <v>33.028599999999997</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 116</v>
+        <v xml:space="preserve"> 108</v>
       </c>
       <c r="H56" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 34485</v>
+        <v xml:space="preserve"> 51590</v>
       </c>
       <c r="I56" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  4302</v>
+        <v xml:space="preserve"> 12024</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2194,28 +2187,28 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D57">
-        <v>956</v>
+        <v>966</v>
       </c>
       <c r="E57">
-        <v>12.7006</v>
+        <v>12.6288</v>
       </c>
       <c r="F57">
-        <v>11.647</v>
+        <v>11.818199999999999</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 115</v>
+        <v xml:space="preserve"> 116</v>
       </c>
       <c r="H57" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 34681</v>
+        <v xml:space="preserve"> 34485</v>
       </c>
       <c r="I57" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  4240</v>
+        <v xml:space="preserve">  4302</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2226,28 +2219,28 @@
         <v>0</v>
       </c>
       <c r="C58">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D58">
-        <v>879</v>
+        <v>956</v>
       </c>
       <c r="E58">
-        <v>12.7278</v>
+        <v>12.7006</v>
       </c>
       <c r="F58">
-        <v>11.5527</v>
+        <v>11.647</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 107</v>
+        <v xml:space="preserve"> 115</v>
       </c>
       <c r="H58" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 34755</v>
+        <v xml:space="preserve"> 34681</v>
       </c>
       <c r="I58" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  4206</v>
+        <v xml:space="preserve">  4240</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2258,112 +2251,112 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D59">
-        <v>965</v>
+        <v>879</v>
       </c>
       <c r="E59">
-        <v>12.3652</v>
+        <v>12.7278</v>
       </c>
       <c r="F59">
-        <v>4.4736000000000002</v>
+        <v>11.5527</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 116</v>
+        <v xml:space="preserve"> 107</v>
       </c>
       <c r="H59" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 33765</v>
+        <v xml:space="preserve"> 34755</v>
       </c>
       <c r="I59" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  1628</v>
+        <v xml:space="preserve">  4206</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="B60">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C60">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D60">
-        <v>739</v>
+        <v>965</v>
       </c>
       <c r="E60">
-        <v>17.020199999999999</v>
+        <v>12.3652</v>
       </c>
       <c r="F60">
-        <v>-30.112400000000001</v>
+        <v>4.4736000000000002</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  93</v>
+        <v xml:space="preserve"> 116</v>
       </c>
       <c r="H60" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 46476</v>
+        <v xml:space="preserve"> 33765</v>
       </c>
       <c r="I60" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>-10963</v>
+        <v xml:space="preserve">  1628</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C61">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D61">
-        <v>859</v>
+        <v>739</v>
       </c>
       <c r="E61">
-        <v>13.2637</v>
+        <v>17.020199999999999</v>
       </c>
       <c r="F61">
-        <v>42.029299999999999</v>
+        <v>-30.112400000000001</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 105</v>
+        <v xml:space="preserve">  93</v>
       </c>
       <c r="H61" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 36218</v>
+        <v xml:space="preserve"> 46476</v>
       </c>
       <c r="I61" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> 15301</v>
+        <v>-10963</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="C62">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D62">
-        <v>852</v>
+        <v>859</v>
       </c>
       <c r="E62">
-        <v>12.945499999999999</v>
+        <v>13.2637</v>
       </c>
       <c r="F62">
-        <v>21.683</v>
+        <v>42.029299999999999</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="0"/>
@@ -2371,43 +2364,43 @@
       </c>
       <c r="H62" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 35349</v>
+        <v xml:space="preserve"> 36218</v>
       </c>
       <c r="I62" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  7894</v>
+        <v xml:space="preserve"> 15301</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="C63">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D63">
-        <v>932</v>
+        <v>852</v>
       </c>
       <c r="E63">
-        <v>11.3155</v>
+        <v>12.945499999999999</v>
       </c>
       <c r="F63">
-        <v>13.0924</v>
+        <v>21.683</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 113</v>
+        <v xml:space="preserve"> 105</v>
       </c>
       <c r="H63" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 30898</v>
+        <v xml:space="preserve"> 35349</v>
       </c>
       <c r="I63" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  4766</v>
+        <v xml:space="preserve">  7894</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2418,124 +2411,124 @@
         <v>0</v>
       </c>
       <c r="C64">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D64">
-        <v>892</v>
+        <v>932</v>
       </c>
       <c r="E64">
-        <v>11.3375</v>
+        <v>11.3155</v>
       </c>
       <c r="F64">
-        <v>12.9915</v>
+        <v>13.0924</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 109</v>
+        <v xml:space="preserve"> 113</v>
       </c>
       <c r="H64" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 30958</v>
+        <v xml:space="preserve"> 30898</v>
       </c>
       <c r="I64" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  4729</v>
+        <v xml:space="preserve">  4766</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D65">
-        <v>690</v>
+        <v>892</v>
       </c>
       <c r="E65">
-        <v>8.8556000000000008</v>
+        <v>11.3375</v>
       </c>
       <c r="F65">
-        <v>11.8119</v>
+        <v>12.9915</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  89</v>
+        <v xml:space="preserve"> 109</v>
       </c>
       <c r="H65" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 24181</v>
+        <v xml:space="preserve"> 30958</v>
       </c>
       <c r="I65" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  4300</v>
+        <v xml:space="preserve">  4729</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B66">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C66">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D66">
-        <v>796</v>
+        <v>690</v>
       </c>
       <c r="E66">
-        <v>12.6578</v>
+        <v>8.8556000000000008</v>
       </c>
       <c r="F66">
-        <v>-26.742999999999999</v>
+        <v>11.8119</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" ref="G66:G107" si="3">RIGHT("              "&amp;TRUNC((D66+200)/10),4)</f>
-        <v xml:space="preserve">  99</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  89</v>
       </c>
       <c r="H66" s="2" t="str">
-        <f t="shared" ref="H66:H107" si="4">RIGHT("              " &amp;TRUNC(E66*65536 / 24),6)</f>
-        <v xml:space="preserve"> 34564</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> 24181</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f t="shared" ref="I66:I107" si="5">RIGHT("              " &amp; TRUNC(F66*32767 / 90),6)</f>
-        <v xml:space="preserve"> -9736</v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  4300</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="B67">
         <v>8</v>
       </c>
       <c r="C67">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D67">
-        <v>831</v>
+        <v>796</v>
       </c>
       <c r="E67">
-        <v>18.523099999999999</v>
+        <v>12.6578</v>
       </c>
       <c r="F67">
-        <v>-32.347999999999999</v>
+        <v>-26.742999999999999</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 103</v>
+        <f t="shared" ref="G67:G109" si="3">RIGHT("              "&amp;TRUNC((D67+200)/10),4)</f>
+        <v xml:space="preserve">  99</v>
       </c>
       <c r="H67" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 50580</v>
+        <f t="shared" ref="H67:H109" si="4">RIGHT("              " &amp;TRUNC(E67*65536 / 24),6)</f>
+        <v xml:space="preserve"> 34564</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>-11777</v>
+        <f t="shared" ref="I67:I109" si="5">RIGHT("              " &amp; TRUNC(F67*32767 / 90),6)</f>
+        <v xml:space="preserve"> -9736</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2546,92 +2539,92 @@
         <v>8</v>
       </c>
       <c r="C68">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D68">
-        <v>906</v>
+        <v>831</v>
       </c>
       <c r="E68">
-        <v>18.720199999999998</v>
+        <v>18.523099999999999</v>
       </c>
       <c r="F68">
-        <v>-32.291899999999998</v>
+        <v>-32.347999999999999</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 110</v>
+        <v xml:space="preserve"> 103</v>
       </c>
       <c r="H68" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 51118</v>
+        <v xml:space="preserve"> 50580</v>
       </c>
       <c r="I68" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>-11756</v>
+        <v>-11777</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B69">
         <v>8</v>
       </c>
       <c r="C69">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D69">
-        <v>610</v>
+        <v>906</v>
       </c>
       <c r="E69">
-        <v>19.896100000000001</v>
+        <v>18.720199999999998</v>
       </c>
       <c r="F69">
-        <v>18.778400000000001</v>
+        <v>-32.291899999999998</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">  81</v>
+        <v xml:space="preserve"> 110</v>
       </c>
       <c r="H69" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 54329</v>
+        <v xml:space="preserve"> 51118</v>
       </c>
       <c r="I69" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  6836</v>
+        <v>-11756</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B70">
         <v>8</v>
       </c>
       <c r="C70">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D70">
-        <v>896</v>
+        <v>610</v>
       </c>
       <c r="E70">
-        <v>20.891100000000002</v>
+        <v>19.896100000000001</v>
       </c>
       <c r="F70">
-        <v>-12.537100000000001</v>
+        <v>18.778400000000001</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 109</v>
+        <v xml:space="preserve">  81</v>
       </c>
       <c r="H70" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 57046</v>
+        <v xml:space="preserve"> 54329</v>
       </c>
       <c r="I70" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> -4564</v>
+        <v xml:space="preserve">  6836</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -2639,19 +2632,19 @@
         <v>4</v>
       </c>
       <c r="B71">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C71">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D71">
-        <v>890</v>
+        <v>896</v>
       </c>
       <c r="E71">
-        <v>20.982199999999999</v>
+        <v>20.891100000000002</v>
       </c>
       <c r="F71">
-        <v>-12.6355</v>
+        <v>-12.537100000000001</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="3"/>
@@ -2659,267 +2652,267 @@
       </c>
       <c r="H71" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 57295</v>
+        <v xml:space="preserve"> 57046</v>
       </c>
       <c r="I71" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> -4600</v>
+        <v xml:space="preserve"> -4564</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C72">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D72">
-        <v>946</v>
+        <v>890</v>
       </c>
       <c r="E72">
-        <v>1.6115999999999999</v>
+        <v>20.982199999999999</v>
       </c>
       <c r="F72">
-        <v>15.7837</v>
+        <v>-12.6355</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 114</v>
+        <v xml:space="preserve"> 109</v>
       </c>
       <c r="H72" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  4400</v>
+        <v xml:space="preserve"> 57295</v>
       </c>
       <c r="I72" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  5746</v>
+        <v xml:space="preserve"> -4600</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B73">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C73">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D73">
-        <v>826</v>
+        <v>946</v>
       </c>
       <c r="E73">
-        <v>20.101299999999998</v>
+        <v>1.6115999999999999</v>
       </c>
       <c r="F73">
-        <v>-21.9222</v>
+        <v>15.7837</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 102</v>
+        <v xml:space="preserve"> 114</v>
       </c>
       <c r="H73" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 54889</v>
+        <v xml:space="preserve">  4400</v>
       </c>
       <c r="I73" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> -7981</v>
+        <v xml:space="preserve">  5746</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B74">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C74">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D74">
-        <v>1010</v>
+        <v>826</v>
       </c>
       <c r="E74">
-        <v>1.7055</v>
+        <v>20.101299999999998</v>
       </c>
       <c r="F74">
-        <v>51.575499999999998</v>
+        <v>-21.9222</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 121</v>
+        <v xml:space="preserve"> 102</v>
       </c>
       <c r="H74" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  4657</v>
+        <v xml:space="preserve"> 54889</v>
       </c>
       <c r="I74" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> 18777</v>
+        <v xml:space="preserve"> -7981</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C75">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D75">
-        <v>887</v>
+        <v>1010</v>
       </c>
       <c r="E75">
-        <v>2.7113</v>
+        <v>1.7055</v>
       </c>
       <c r="F75">
-        <v>-1.3299999999999999E-2</v>
+        <v>51.575499999999998</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 108</v>
+        <v xml:space="preserve"> 121</v>
       </c>
       <c r="H75" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  7403</v>
+        <v xml:space="preserve">  4657</v>
       </c>
       <c r="I75" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    -4</v>
+        <v xml:space="preserve"> 18777</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B76">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C76">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D76">
-        <v>800</v>
+        <v>887</v>
       </c>
       <c r="E76">
-        <v>5.7793999999999999</v>
+        <v>2.7113</v>
       </c>
       <c r="F76">
-        <v>7.9299999999999995E-2</v>
+        <v>-1.3299999999999999E-2</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 100</v>
+        <v xml:space="preserve"> 108</v>
       </c>
       <c r="H76" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 15781</v>
+        <v xml:space="preserve">  7403</v>
       </c>
       <c r="I76" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    28</v>
+        <v xml:space="preserve">    -4</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B77">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C77">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D77">
-        <v>816</v>
+        <v>800</v>
       </c>
       <c r="E77">
-        <v>5.4028999999999998</v>
+        <v>5.7793999999999999</v>
       </c>
       <c r="F77">
-        <v>-24.5242</v>
+        <v>7.9299999999999995E-2</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 101</v>
+        <v xml:space="preserve"> 100</v>
       </c>
       <c r="H77" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 14753</v>
+        <v xml:space="preserve"> 15781</v>
       </c>
       <c r="I77" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> -8928</v>
+        <v xml:space="preserve">    28</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="B78">
         <v>8</v>
       </c>
       <c r="C78">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D78">
-        <v>730</v>
+        <v>816</v>
       </c>
       <c r="E78">
-        <v>16.283999999999999</v>
+        <v>5.4028999999999998</v>
       </c>
       <c r="F78">
-        <v>-22.975100000000001</v>
+        <v>-24.5242</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">  93</v>
+        <v xml:space="preserve"> 101</v>
       </c>
       <c r="H78" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 44466</v>
+        <v xml:space="preserve"> 14753</v>
       </c>
       <c r="I78" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> -8364</v>
+        <v xml:space="preserve"> -8928</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C79">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D79">
-        <v>694</v>
+        <v>730</v>
       </c>
       <c r="E79">
-        <v>9.9259000000000004</v>
+        <v>16.283999999999999</v>
       </c>
       <c r="F79">
-        <v>69.065299999999993</v>
+        <v>-22.975100000000001</v>
       </c>
       <c r="G79" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">  89</v>
+        <v xml:space="preserve">  93</v>
       </c>
       <c r="H79" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 27104</v>
+        <v xml:space="preserve"> 44466</v>
       </c>
       <c r="I79" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> 25145</v>
+        <v xml:space="preserve"> -8364</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -2930,156 +2923,156 @@
         <v>0</v>
       </c>
       <c r="C80">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D80">
-        <v>841</v>
+        <v>694</v>
       </c>
       <c r="E80">
-        <v>9.9313000000000002</v>
+        <v>9.9259000000000004</v>
       </c>
       <c r="F80">
-        <v>69.679400000000001</v>
+        <v>69.065299999999993</v>
       </c>
       <c r="G80" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 104</v>
+        <v xml:space="preserve">  89</v>
       </c>
       <c r="H80" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 27119</v>
+        <v xml:space="preserve"> 27104</v>
       </c>
       <c r="I80" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> 25368</v>
+        <v xml:space="preserve"> 25145</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="B81">
         <v>0</v>
       </c>
       <c r="C81">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D81">
-        <v>752</v>
+        <v>841</v>
       </c>
       <c r="E81">
-        <v>13.616899999999999</v>
+        <v>9.9313000000000002</v>
       </c>
       <c r="F81">
-        <v>-29.865400000000001</v>
+        <v>69.679400000000001</v>
       </c>
       <c r="G81" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">  95</v>
+        <v xml:space="preserve"> 104</v>
       </c>
       <c r="H81" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 37183</v>
+        <v xml:space="preserve"> 27119</v>
       </c>
       <c r="I81" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>-10873</v>
+        <v xml:space="preserve"> 25368</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
       <c r="C82">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D82">
-        <v>1049</v>
+        <v>752</v>
       </c>
       <c r="E82">
-        <v>12.4177</v>
+        <v>13.616899999999999</v>
       </c>
       <c r="F82">
-        <v>12.887</v>
+        <v>-29.865400000000001</v>
       </c>
       <c r="G82" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 124</v>
+        <v xml:space="preserve">  95</v>
       </c>
       <c r="H82" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 33908</v>
+        <v xml:space="preserve"> 37183</v>
       </c>
       <c r="I82" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  4691</v>
+        <v>-10873</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="B83">
         <v>0</v>
       </c>
       <c r="C83">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D83">
-        <v>905</v>
+        <v>1049</v>
       </c>
       <c r="E83">
-        <v>12.423400000000001</v>
+        <v>12.4177</v>
       </c>
       <c r="F83">
-        <v>18.191500000000001</v>
+        <v>12.887</v>
       </c>
       <c r="G83" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 110</v>
+        <v xml:space="preserve"> 124</v>
       </c>
       <c r="H83" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 33924</v>
+        <v xml:space="preserve"> 33908</v>
       </c>
       <c r="I83" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  6623</v>
+        <v xml:space="preserve">  4691</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
+        <v>24</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
         <v>85</v>
       </c>
-      <c r="B84">
-        <v>0</v>
-      </c>
-      <c r="C84">
-        <v>86</v>
-      </c>
       <c r="D84">
-        <v>890</v>
+        <v>905</v>
       </c>
       <c r="E84">
-        <v>12.4366</v>
+        <v>12.423400000000001</v>
       </c>
       <c r="F84">
-        <v>12.946199999999999</v>
+        <v>18.191500000000001</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 109</v>
+        <v xml:space="preserve"> 110</v>
       </c>
       <c r="H84" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 33960</v>
+        <v xml:space="preserve"> 33924</v>
       </c>
       <c r="I84" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  4713</v>
+        <v xml:space="preserve">  6623</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -3090,92 +3083,92 @@
         <v>0</v>
       </c>
       <c r="C85">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D85">
-        <v>863</v>
+        <v>890</v>
       </c>
       <c r="E85">
-        <v>12.5137</v>
+        <v>12.4366</v>
       </c>
       <c r="F85">
-        <v>12.3911</v>
+        <v>12.946199999999999</v>
       </c>
       <c r="G85" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 106</v>
+        <v xml:space="preserve"> 109</v>
       </c>
       <c r="H85" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 34170</v>
+        <v xml:space="preserve"> 33960</v>
       </c>
       <c r="I85" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  4511</v>
+        <v xml:space="preserve">  4713</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
       <c r="C86">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D86">
-        <v>1318</v>
+        <v>863</v>
       </c>
       <c r="E86">
-        <v>12.533099999999999</v>
+        <v>12.5137</v>
       </c>
       <c r="F86">
-        <v>14.420400000000001</v>
+        <v>12.3911</v>
       </c>
       <c r="G86" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 151</v>
+        <v xml:space="preserve"> 106</v>
       </c>
       <c r="H86" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 34223</v>
+        <v xml:space="preserve"> 34170</v>
       </c>
       <c r="I86" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  5250</v>
+        <v xml:space="preserve">  4511</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="C87">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D87">
-        <v>975</v>
+        <v>1318</v>
       </c>
       <c r="E87">
-        <v>12.5944</v>
+        <v>12.533099999999999</v>
       </c>
       <c r="F87">
-        <v>12.5563</v>
+        <v>14.420400000000001</v>
       </c>
       <c r="G87" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 117</v>
+        <v xml:space="preserve"> 151</v>
       </c>
       <c r="H87" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 34391</v>
+        <v xml:space="preserve"> 34223</v>
       </c>
       <c r="I87" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  4571</v>
+        <v xml:space="preserve">  5250</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3186,188 +3179,188 @@
         <v>0</v>
       </c>
       <c r="C88">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D88">
-        <v>954</v>
+        <v>975</v>
       </c>
       <c r="E88">
-        <v>12.613799999999999</v>
+        <v>12.5944</v>
       </c>
       <c r="F88">
-        <v>13.1629</v>
+        <v>12.5563</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 115</v>
+        <v xml:space="preserve"> 117</v>
       </c>
       <c r="H88" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 34444</v>
+        <v xml:space="preserve"> 34391</v>
       </c>
       <c r="I88" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  4792</v>
+        <v xml:space="preserve">  4571</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="B89">
         <v>0</v>
       </c>
       <c r="C89">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D89">
-        <v>1357</v>
+        <v>954</v>
       </c>
       <c r="E89">
-        <v>12.5907</v>
+        <v>12.613799999999999</v>
       </c>
       <c r="F89">
-        <v>14.4963</v>
+        <v>13.1629</v>
       </c>
       <c r="G89" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 155</v>
+        <v xml:space="preserve"> 115</v>
       </c>
       <c r="H89" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 34381</v>
+        <v xml:space="preserve"> 34444</v>
       </c>
       <c r="I89" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  5277</v>
+        <v xml:space="preserve">  4792</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B90">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C90">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D90">
-        <v>652</v>
+        <v>1357</v>
       </c>
       <c r="E90">
-        <v>17.285399999999999</v>
+        <v>12.5907</v>
       </c>
       <c r="F90">
-        <v>43.136499999999998</v>
+        <v>14.4963</v>
       </c>
       <c r="G90" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">  85</v>
+        <v xml:space="preserve"> 155</v>
       </c>
       <c r="H90" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 47200</v>
+        <v xml:space="preserve"> 34381</v>
       </c>
       <c r="I90" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> 15705</v>
+        <v xml:space="preserve">  5277</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C91">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D91">
-        <v>620</v>
+        <v>652</v>
       </c>
       <c r="E91">
-        <v>7.7415000000000003</v>
+        <v>17.285399999999999</v>
       </c>
       <c r="F91">
-        <v>-23.853100000000001</v>
+        <v>43.136499999999998</v>
       </c>
       <c r="G91" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">  82</v>
+        <v xml:space="preserve">  85</v>
       </c>
       <c r="H91" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 21139</v>
+        <v xml:space="preserve"> 47200</v>
       </c>
       <c r="I91" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> -8684</v>
+        <v xml:space="preserve"> 15705</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C92">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D92">
-        <v>824</v>
+        <v>620</v>
       </c>
       <c r="E92">
-        <v>12.848100000000001</v>
+        <v>7.7415000000000003</v>
       </c>
       <c r="F92">
-        <v>41.120399999999997</v>
+        <v>-23.853100000000001</v>
       </c>
       <c r="G92" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 102</v>
+        <v xml:space="preserve">  82</v>
       </c>
       <c r="H92" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 35083</v>
+        <v xml:space="preserve"> 21139</v>
       </c>
       <c r="I92" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> 14971</v>
+        <v xml:space="preserve"> -8684</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B93">
         <v>0</v>
       </c>
       <c r="C93">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D93">
-        <v>973</v>
+        <v>824</v>
       </c>
       <c r="E93">
-        <v>10.732699999999999</v>
+        <v>12.848100000000001</v>
       </c>
       <c r="F93">
-        <v>11.703799999999999</v>
+        <v>41.120399999999997</v>
       </c>
       <c r="G93" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 117</v>
+        <v xml:space="preserve"> 102</v>
       </c>
       <c r="H93" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 29307</v>
+        <v xml:space="preserve"> 35083</v>
       </c>
       <c r="I93" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  4261</v>
+        <v xml:space="preserve"> 14971</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -3378,92 +3371,92 @@
         <v>0</v>
       </c>
       <c r="C94">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D94">
-        <v>925</v>
+        <v>973</v>
       </c>
       <c r="E94">
-        <v>10.779400000000001</v>
+        <v>10.732699999999999</v>
       </c>
       <c r="F94">
-        <v>11.819900000000001</v>
+        <v>11.703799999999999</v>
       </c>
       <c r="G94" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 112</v>
+        <v xml:space="preserve"> 117</v>
       </c>
       <c r="H94" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 29434</v>
+        <v xml:space="preserve"> 29307</v>
       </c>
       <c r="I94" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  4303</v>
+        <v xml:space="preserve">  4261</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="B95">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C95">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D95">
-        <v>990</v>
+        <v>925</v>
       </c>
       <c r="E95">
-        <v>11.246600000000001</v>
+        <v>10.779400000000001</v>
       </c>
       <c r="F95">
-        <v>55.018999999999998</v>
+        <v>11.819900000000001</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 119</v>
+        <v xml:space="preserve"> 112</v>
       </c>
       <c r="H95" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 30710</v>
+        <v xml:space="preserve"> 29434</v>
       </c>
       <c r="I95" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> 20031</v>
+        <v xml:space="preserve">  4303</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C96">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D96">
-        <v>1014</v>
+        <v>990</v>
       </c>
       <c r="E96">
-        <v>12.2301</v>
+        <v>11.246600000000001</v>
       </c>
       <c r="F96">
-        <v>14.9003</v>
+        <v>55.018999999999998</v>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 121</v>
+        <v xml:space="preserve"> 119</v>
       </c>
       <c r="H96" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 33396</v>
+        <v xml:space="preserve"> 30710</v>
       </c>
       <c r="I96" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  5424</v>
+        <v xml:space="preserve"> 20031</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -3474,28 +3467,28 @@
         <v>0</v>
       </c>
       <c r="C97">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D97">
-        <v>987</v>
+        <v>1014</v>
       </c>
       <c r="E97">
-        <v>12.313800000000001</v>
+        <v>12.2301</v>
       </c>
       <c r="F97">
-        <v>14.416499999999999</v>
+        <v>14.9003</v>
       </c>
       <c r="G97" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 118</v>
+        <v xml:space="preserve"> 121</v>
       </c>
       <c r="H97" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 33624</v>
+        <v xml:space="preserve"> 33396</v>
       </c>
       <c r="I97" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  5248</v>
+        <v xml:space="preserve">  5424</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -3506,314 +3499,375 @@
         <v>0</v>
       </c>
       <c r="C98">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D98">
-        <v>935</v>
+        <v>987</v>
       </c>
       <c r="E98">
-        <v>12.3819</v>
+        <v>12.313800000000001</v>
       </c>
       <c r="F98">
-        <v>15.8218</v>
+        <v>14.416499999999999</v>
       </c>
       <c r="G98" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 113</v>
+        <v xml:space="preserve"> 118</v>
       </c>
       <c r="H98" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 33810</v>
+        <v xml:space="preserve"> 33624</v>
       </c>
       <c r="I98" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  5760</v>
+        <v xml:space="preserve">  5248</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="B99">
         <v>0</v>
       </c>
       <c r="C99">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D99">
-        <v>786</v>
+        <v>935</v>
       </c>
       <c r="E99">
-        <v>14.0535</v>
+        <v>12.3819</v>
       </c>
       <c r="F99">
-        <v>54.3489</v>
+        <v>15.8218</v>
       </c>
       <c r="G99" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">  98</v>
+        <v xml:space="preserve"> 113</v>
       </c>
       <c r="H99" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 38375</v>
+        <v xml:space="preserve"> 33810</v>
       </c>
       <c r="I99" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> 19787</v>
+        <v xml:space="preserve">  5760</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C100">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D100">
-        <v>740</v>
+        <v>786</v>
       </c>
       <c r="E100">
-        <v>1.5561</v>
+        <v>14.0535</v>
       </c>
       <c r="F100">
-        <v>60.658000000000001</v>
+        <v>54.3489</v>
       </c>
       <c r="G100" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">  94</v>
+        <v xml:space="preserve">  98</v>
       </c>
       <c r="H100" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  4249</v>
+        <v xml:space="preserve"> 38375</v>
       </c>
       <c r="I100" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> 22084</v>
+        <v xml:space="preserve"> 19787</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>29</v>
-      </c>
       <c r="B101">
         <v>0</v>
       </c>
       <c r="C101">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D101">
-        <v>800</v>
+        <v>989</v>
       </c>
       <c r="E101">
-        <v>12.666499999999999</v>
+        <v>15.1079583</v>
       </c>
       <c r="F101">
-        <v>-11.623100000000001</v>
+        <v>55.765555550000002</v>
       </c>
       <c r="G101" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 100</v>
+        <v xml:space="preserve"> 118</v>
       </c>
       <c r="H101" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 34587</v>
+        <v xml:space="preserve"> 41254</v>
       </c>
       <c r="I101" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> -4231</v>
+        <v xml:space="preserve"> 20302</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C102">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D102">
-        <v>976</v>
+        <v>740</v>
       </c>
       <c r="E102">
-        <v>10.7971</v>
+        <v>1.5561</v>
       </c>
       <c r="F102">
-        <v>12.5816</v>
+        <v>60.658000000000001</v>
       </c>
       <c r="G102" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 117</v>
+        <v xml:space="preserve">  94</v>
       </c>
       <c r="H102" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 29483</v>
+        <v xml:space="preserve">  4249</v>
       </c>
       <c r="I102" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">  4580</v>
+        <v xml:space="preserve"> 22084</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
       <c r="C103">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D103">
-        <v>841</v>
+        <v>800</v>
       </c>
       <c r="E103">
-        <v>12.316000000000001</v>
+        <v>12.666499999999999</v>
       </c>
       <c r="F103">
-        <v>47.304000000000002</v>
+        <v>-11.623100000000001</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 104</v>
+        <v xml:space="preserve"> 100</v>
       </c>
       <c r="H103" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 33630</v>
+        <v xml:space="preserve"> 34587</v>
       </c>
       <c r="I103" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> 17222</v>
+        <v xml:space="preserve"> -4231</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B104">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C104">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D104">
-        <v>885</v>
+        <v>976</v>
       </c>
       <c r="E104">
-        <v>16.542200000000001</v>
+        <v>10.7971</v>
       </c>
       <c r="F104">
-        <v>-13.053599999999999</v>
+        <v>12.5816</v>
       </c>
       <c r="G104" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 108</v>
+        <v xml:space="preserve"> 117</v>
       </c>
       <c r="H104" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 45171</v>
+        <v xml:space="preserve"> 29483</v>
       </c>
       <c r="I104" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> -4752</v>
+        <v xml:space="preserve">  4580</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="B105">
         <v>0</v>
       </c>
       <c r="C105">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D105">
-        <v>1006</v>
+        <v>841</v>
       </c>
       <c r="E105">
-        <v>11.1919</v>
+        <v>12.316000000000001</v>
       </c>
       <c r="F105">
-        <v>55.674100000000003</v>
+        <v>47.304000000000002</v>
       </c>
       <c r="G105" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 120</v>
+        <v xml:space="preserve"> 104</v>
       </c>
       <c r="H105" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 30561</v>
+        <v xml:space="preserve"> 33630</v>
       </c>
       <c r="I105" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> 20269</v>
+        <v xml:space="preserve"> 17222</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="B106">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C106">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D106">
-        <v>988</v>
+        <v>885</v>
       </c>
       <c r="E106">
-        <v>11.96</v>
+        <v>16.542200000000001</v>
       </c>
       <c r="F106">
-        <v>53.374499999999998</v>
+        <v>-13.053599999999999</v>
       </c>
       <c r="G106" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 118</v>
+        <v xml:space="preserve"> 108</v>
       </c>
       <c r="H106" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 32658</v>
+        <v xml:space="preserve"> 45171</v>
       </c>
       <c r="I106" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> 19432</v>
+        <v xml:space="preserve"> -4752</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="B107">
         <v>0</v>
       </c>
       <c r="C107">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D107">
-        <v>807</v>
+        <v>1006</v>
       </c>
       <c r="E107">
-        <v>0.67279999999999995</v>
+        <v>11.1919</v>
       </c>
       <c r="F107">
-        <v>41.685299999999998</v>
+        <v>55.674100000000003</v>
       </c>
       <c r="G107" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> 100</v>
+        <v xml:space="preserve"> 120</v>
       </c>
       <c r="H107" s="2" t="str">
         <f t="shared" si="4"/>
+        <v xml:space="preserve"> 30561</v>
+      </c>
+      <c r="I107" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> 20269</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>82</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>109</v>
+      </c>
+      <c r="D108">
+        <v>988</v>
+      </c>
+      <c r="E108">
+        <v>11.96</v>
+      </c>
+      <c r="F108">
+        <v>53.374499999999998</v>
+      </c>
+      <c r="G108" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> 118</v>
+      </c>
+      <c r="H108" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> 32658</v>
+      </c>
+      <c r="I108" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> 19432</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>0</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>110</v>
+      </c>
+      <c r="D109">
+        <v>807</v>
+      </c>
+      <c r="E109">
+        <v>0.67279999999999995</v>
+      </c>
+      <c r="F109">
+        <v>41.685299999999998</v>
+      </c>
+      <c r="G109" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> 100</v>
+      </c>
+      <c r="H109" s="2" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">  1837</v>
       </c>
-      <c r="I107" s="1" t="str">
+      <c r="I109" s="1" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> 15176</v>
       </c>
@@ -16259,7 +16313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68D0565-DCC6-40E3-9DC5-8D3FD09BF76B}">
   <dimension ref="A1:H408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A392" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H392" sqref="H392"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add missing magnitude to Herschel catalog
</commit_message>
<xml_diff>
--- a/SmartHandController/Catalog.xlsx
+++ b/SmartHandController/Catalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\GitHub\TeenAstro\SmartHandController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE276AA-FC81-4AF5-828F-B6EE1D235975}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E474F98-35F8-4B11-9A8A-F396EA4D0DE6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{983D245A-AE43-4906-82C2-4606C1D254C7}"/>
+    <workbookView xWindow="165" yWindow="555" windowWidth="12735" windowHeight="11955" activeTab="1" xr2:uid="{983D245A-AE43-4906-82C2-4606C1D254C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Messier" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="00000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -60,10 +61,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -380,8 +382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{942127E5-A596-4E77-AF44-2F423C350B23}">
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101:F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3597,10 +3599,10 @@
       <c r="D101">
         <v>989</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="3">
         <v>15.1079583</v>
       </c>
-      <c r="F101">
+      <c r="F101" s="3">
         <v>55.765555550000002</v>
       </c>
       <c r="G101" t="str">
@@ -3882,8 +3884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209E9D4A-E466-4952-AE11-D2E91569FD33}">
   <dimension ref="A1:I388"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3963,7 +3965,7 @@
         <v>136</v>
       </c>
       <c r="D3">
-        <v>9990</v>
+        <v>1230</v>
       </c>
       <c r="E3">
         <v>0.5252</v>
@@ -3973,7 +3975,7 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 143</v>
       </c>
       <c r="H3" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4219,7 +4221,7 @@
         <v>278</v>
       </c>
       <c r="D11">
-        <v>9990</v>
+        <v>1070</v>
       </c>
       <c r="E11">
         <v>0.8679</v>
@@ -4229,7 +4231,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 127</v>
       </c>
       <c r="H11" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4411,7 +4413,7 @@
         <v>488</v>
       </c>
       <c r="D17">
-        <v>9990</v>
+        <v>1040</v>
       </c>
       <c r="E17">
         <v>1.363</v>
@@ -4421,7 +4423,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 124</v>
       </c>
       <c r="H17" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4443,7 +4445,7 @@
         <v>524</v>
       </c>
       <c r="D18">
-        <v>9990</v>
+        <v>1040</v>
       </c>
       <c r="E18">
         <v>1.4133</v>
@@ -4453,7 +4455,7 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 124</v>
       </c>
       <c r="H18" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4539,7 +4541,7 @@
         <v>596</v>
       </c>
       <c r="D21">
-        <v>9990</v>
+        <v>1090</v>
       </c>
       <c r="E21">
         <v>1.5478000000000001</v>
@@ -4549,7 +4551,7 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 129</v>
       </c>
       <c r="H21" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4635,7 +4637,7 @@
         <v>615</v>
       </c>
       <c r="D24">
-        <v>9990</v>
+        <v>1170</v>
       </c>
       <c r="E24">
         <v>1.5849</v>
@@ -4645,7 +4647,7 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 137</v>
       </c>
       <c r="H24" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4795,7 +4797,7 @@
         <v>720</v>
       </c>
       <c r="D29">
-        <v>9990</v>
+        <v>1020</v>
       </c>
       <c r="E29">
         <v>1.8835</v>
@@ -4805,7 +4807,7 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 122</v>
       </c>
       <c r="H29" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4891,7 +4893,7 @@
         <v>779</v>
       </c>
       <c r="D32">
-        <v>9990</v>
+        <v>1120</v>
       </c>
       <c r="E32">
         <v>1.9951000000000001</v>
@@ -4901,7 +4903,7 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 132</v>
       </c>
       <c r="H32" s="2" t="str">
         <f t="shared" si="1"/>
@@ -5051,7 +5053,7 @@
         <v>936</v>
       </c>
       <c r="D37">
-        <v>9990</v>
+        <v>1020</v>
       </c>
       <c r="E37">
         <v>2.4603999999999999</v>
@@ -5061,7 +5063,7 @@
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 122</v>
       </c>
       <c r="H37" s="2" t="str">
         <f t="shared" si="1"/>
@@ -5659,7 +5661,7 @@
         <v>1788</v>
       </c>
       <c r="D56">
-        <v>9990</v>
+        <v>600</v>
       </c>
       <c r="E56">
         <v>5.1147999999999998</v>
@@ -5669,7 +5671,7 @@
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
-        <v>1019</v>
+        <v xml:space="preserve">  80</v>
       </c>
       <c r="H56" s="2" t="str">
         <f t="shared" si="1"/>
@@ -5915,7 +5917,7 @@
         <v>1999</v>
       </c>
       <c r="D64">
-        <v>9990</v>
+        <v>1100</v>
       </c>
       <c r="E64">
         <v>5.6070000000000002</v>
@@ -5925,7 +5927,7 @@
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 130</v>
       </c>
       <c r="H64" s="2" t="str">
         <f t="shared" si="1"/>
@@ -5979,7 +5981,7 @@
         <v>2024</v>
       </c>
       <c r="D66">
-        <v>9990</v>
+        <v>400</v>
       </c>
       <c r="E66">
         <v>5.6951999999999998</v>
@@ -5989,7 +5991,7 @@
       </c>
       <c r="G66" t="str">
         <f t="shared" ref="G66:G129" si="3">RIGHT("              "&amp;TRUNC((D66+200)/10),4)</f>
-        <v>1019</v>
+        <v xml:space="preserve">  60</v>
       </c>
       <c r="H66" s="2" t="str">
         <f t="shared" ref="H66:H129" si="4">RIGHT("              " &amp;TRUNC(E66*65536 / 24),6)</f>
@@ -6011,7 +6013,7 @@
         <v>2126</v>
       </c>
       <c r="D67">
-        <v>9990</v>
+        <v>1020</v>
       </c>
       <c r="E67">
         <v>6.0425000000000004</v>
@@ -6021,7 +6023,7 @@
       </c>
       <c r="G67" t="str">
         <f t="shared" si="3"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 122</v>
       </c>
       <c r="H67" s="2" t="str">
         <f t="shared" si="4"/>
@@ -6139,7 +6141,7 @@
         <v>2185</v>
       </c>
       <c r="D71">
-        <v>9990</v>
+        <v>1000</v>
       </c>
       <c r="E71">
         <v>6.1835000000000004</v>
@@ -6149,7 +6151,7 @@
       </c>
       <c r="G71" t="str">
         <f t="shared" si="3"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 120</v>
       </c>
       <c r="H71" s="2" t="str">
         <f t="shared" si="4"/>
@@ -7643,7 +7645,7 @@
         <v>2742</v>
       </c>
       <c r="D118">
-        <v>9990</v>
+        <v>1140</v>
       </c>
       <c r="E118">
         <v>9.1259999999999994</v>
@@ -7653,7 +7655,7 @@
       </c>
       <c r="G118" t="str">
         <f t="shared" si="3"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 134</v>
       </c>
       <c r="H118" s="2" t="str">
         <f t="shared" si="4"/>
@@ -7803,7 +7805,7 @@
         <v>2811</v>
       </c>
       <c r="D123">
-        <v>9990</v>
+        <v>1140</v>
       </c>
       <c r="E123">
         <v>9.2698</v>
@@ -7813,7 +7815,7 @@
       </c>
       <c r="G123" t="str">
         <f t="shared" si="3"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 134</v>
       </c>
       <c r="H123" s="2" t="str">
         <f t="shared" si="4"/>
@@ -7867,7 +7869,7 @@
         <v>2859</v>
       </c>
       <c r="D125">
-        <v>9990</v>
+        <v>1090</v>
       </c>
       <c r="E125">
         <v>9.4050999999999991</v>
@@ -7877,7 +7879,7 @@
       </c>
       <c r="G125" t="str">
         <f t="shared" si="3"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 129</v>
       </c>
       <c r="H125" s="2" t="str">
         <f t="shared" si="4"/>
@@ -7931,7 +7933,7 @@
         <v>2950</v>
       </c>
       <c r="D127">
-        <v>9990</v>
+        <v>1090</v>
       </c>
       <c r="E127">
         <v>9.7097999999999995</v>
@@ -7941,7 +7943,7 @@
       </c>
       <c r="G127" t="str">
         <f t="shared" si="3"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 129</v>
       </c>
       <c r="H127" s="2" t="str">
         <f t="shared" si="4"/>
@@ -7963,7 +7965,7 @@
         <v>2964</v>
       </c>
       <c r="D128">
-        <v>9990</v>
+        <v>1130</v>
       </c>
       <c r="E128">
         <v>9.7150999999999996</v>
@@ -7973,7 +7975,7 @@
       </c>
       <c r="G128" t="str">
         <f t="shared" si="3"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 133</v>
       </c>
       <c r="H128" s="2" t="str">
         <f t="shared" si="4"/>
@@ -7995,7 +7997,7 @@
         <v>2974</v>
       </c>
       <c r="D129">
-        <v>9990</v>
+        <v>1090</v>
       </c>
       <c r="E129">
         <v>9.7091999999999992</v>
@@ -8005,7 +8007,7 @@
       </c>
       <c r="G129" t="str">
         <f t="shared" si="3"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 129</v>
       </c>
       <c r="H129" s="2" t="str">
         <f t="shared" si="4"/>
@@ -8187,7 +8189,7 @@
         <v>3115</v>
       </c>
       <c r="D135">
-        <v>9990</v>
+        <v>910</v>
       </c>
       <c r="E135">
         <v>10.087199999999999</v>
@@ -8197,7 +8199,7 @@
       </c>
       <c r="G135" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 111</v>
       </c>
       <c r="H135" s="2" t="str">
         <f t="shared" si="7"/>
@@ -8251,7 +8253,7 @@
         <v>3166</v>
       </c>
       <c r="D137">
-        <v>9990</v>
+        <v>1050</v>
       </c>
       <c r="E137">
         <v>10.2293</v>
@@ -8261,7 +8263,7 @@
       </c>
       <c r="G137" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 125</v>
       </c>
       <c r="H137" s="2" t="str">
         <f t="shared" si="7"/>
@@ -8315,7 +8317,7 @@
         <v>3184</v>
       </c>
       <c r="D139">
-        <v>9990</v>
+        <v>960</v>
       </c>
       <c r="E139">
         <v>10.3047</v>
@@ -8325,7 +8327,7 @@
       </c>
       <c r="G139" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 116</v>
       </c>
       <c r="H139" s="2" t="str">
         <f t="shared" si="7"/>
@@ -8507,7 +8509,7 @@
         <v>3245</v>
       </c>
       <c r="D145">
-        <v>9990</v>
+        <v>1070</v>
       </c>
       <c r="E145">
         <v>10.4551</v>
@@ -8517,7 +8519,7 @@
       </c>
       <c r="G145" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 127</v>
       </c>
       <c r="H145" s="2" t="str">
         <f t="shared" si="7"/>
@@ -8571,7 +8573,7 @@
         <v>3294</v>
       </c>
       <c r="D147">
-        <v>9990</v>
+        <v>1120</v>
       </c>
       <c r="E147">
         <v>10.6045</v>
@@ -8581,7 +8583,7 @@
       </c>
       <c r="G147" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 132</v>
       </c>
       <c r="H147" s="2" t="str">
         <f t="shared" si="7"/>
@@ -8795,7 +8797,7 @@
         <v>3414</v>
       </c>
       <c r="D154">
-        <v>9990</v>
+        <v>1090</v>
       </c>
       <c r="E154">
         <v>10.8545</v>
@@ -8805,7 +8807,7 @@
       </c>
       <c r="G154" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 129</v>
       </c>
       <c r="H154" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9019,7 +9021,7 @@
         <v>3593</v>
       </c>
       <c r="D161">
-        <v>9990</v>
+        <v>1100</v>
       </c>
       <c r="E161">
         <v>11.243600000000001</v>
@@ -9029,7 +9031,7 @@
       </c>
       <c r="G161" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 130</v>
       </c>
       <c r="H161" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9083,7 +9085,7 @@
         <v>3608</v>
       </c>
       <c r="D163">
-        <v>9990</v>
+        <v>1070</v>
       </c>
       <c r="E163">
         <v>11.282999999999999</v>
@@ -9093,7 +9095,7 @@
       </c>
       <c r="G163" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 127</v>
       </c>
       <c r="H163" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9115,7 +9117,7 @@
         <v>3610</v>
       </c>
       <c r="D164">
-        <v>9990</v>
+        <v>1070</v>
       </c>
       <c r="E164">
         <v>11.307</v>
@@ -9125,7 +9127,7 @@
       </c>
       <c r="G164" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 127</v>
       </c>
       <c r="H164" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9147,7 +9149,7 @@
         <v>3613</v>
       </c>
       <c r="D165">
-        <v>9990</v>
+        <v>1080</v>
       </c>
       <c r="E165">
         <v>11.31</v>
@@ -9157,7 +9159,7 @@
       </c>
       <c r="G165" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 128</v>
       </c>
       <c r="H165" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9179,7 +9181,7 @@
         <v>3619</v>
       </c>
       <c r="D166">
-        <v>9990</v>
+        <v>1150</v>
       </c>
       <c r="E166">
         <v>11.322699999999999</v>
@@ -9189,7 +9191,7 @@
       </c>
       <c r="G166" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 135</v>
       </c>
       <c r="H166" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9243,7 +9245,7 @@
         <v>3626</v>
       </c>
       <c r="D168">
-        <v>9990</v>
+        <v>1100</v>
       </c>
       <c r="E168">
         <v>11.3344</v>
@@ -9253,7 +9255,7 @@
       </c>
       <c r="G168" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 130</v>
       </c>
       <c r="H168" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9307,7 +9309,7 @@
         <v>3631</v>
       </c>
       <c r="D170">
-        <v>9990</v>
+        <v>1010</v>
       </c>
       <c r="E170">
         <v>11.3508</v>
@@ -9317,7 +9319,7 @@
       </c>
       <c r="G170" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 121</v>
       </c>
       <c r="H170" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9435,7 +9437,7 @@
         <v>3675</v>
       </c>
       <c r="D174">
-        <v>9990</v>
+        <v>1000</v>
       </c>
       <c r="E174">
         <v>11.435700000000001</v>
@@ -9445,7 +9447,7 @@
       </c>
       <c r="G174" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 120</v>
       </c>
       <c r="H174" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9467,7 +9469,7 @@
         <v>3686</v>
       </c>
       <c r="D175">
-        <v>9990</v>
+        <v>1120</v>
       </c>
       <c r="E175">
         <v>11.462199999999999</v>
@@ -9477,7 +9479,7 @@
       </c>
       <c r="G175" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 132</v>
       </c>
       <c r="H175" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9499,7 +9501,7 @@
         <v>3726</v>
       </c>
       <c r="D176">
-        <v>9990</v>
+        <v>1020</v>
       </c>
       <c r="E176">
         <v>11.555899999999999</v>
@@ -9509,7 +9511,7 @@
       </c>
       <c r="G176" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 122</v>
       </c>
       <c r="H176" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9531,7 +9533,7 @@
         <v>3729</v>
       </c>
       <c r="D177">
-        <v>9990</v>
+        <v>1100</v>
       </c>
       <c r="E177">
         <v>11.563700000000001</v>
@@ -9541,7 +9543,7 @@
       </c>
       <c r="G177" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 130</v>
       </c>
       <c r="H177" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9563,7 +9565,7 @@
         <v>3810</v>
       </c>
       <c r="D178">
-        <v>9990</v>
+        <v>1060</v>
       </c>
       <c r="E178">
         <v>11.683</v>
@@ -9573,7 +9575,7 @@
       </c>
       <c r="G178" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 126</v>
       </c>
       <c r="H178" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9595,7 +9597,7 @@
         <v>3813</v>
       </c>
       <c r="D179">
-        <v>9990</v>
+        <v>1150</v>
       </c>
       <c r="E179">
         <v>11.688499999999999</v>
@@ -9605,7 +9607,7 @@
       </c>
       <c r="G179" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 135</v>
       </c>
       <c r="H179" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9627,7 +9629,7 @@
         <v>3877</v>
       </c>
       <c r="D180">
-        <v>9990</v>
+        <v>1120</v>
       </c>
       <c r="E180">
         <v>11.768800000000001</v>
@@ -9637,7 +9639,7 @@
       </c>
       <c r="G180" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 132</v>
       </c>
       <c r="H180" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9691,7 +9693,7 @@
         <v>3898</v>
       </c>
       <c r="D182">
-        <v>9990</v>
+        <v>1080</v>
       </c>
       <c r="E182">
         <v>11.8209</v>
@@ -9701,7 +9703,7 @@
       </c>
       <c r="G182" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 128</v>
       </c>
       <c r="H182" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9723,7 +9725,7 @@
         <v>3900</v>
       </c>
       <c r="D183">
-        <v>9990</v>
+        <v>110</v>
       </c>
       <c r="E183">
         <v>11.8193</v>
@@ -9733,7 +9735,7 @@
       </c>
       <c r="G183" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve">  31</v>
       </c>
       <c r="H183" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9819,7 +9821,7 @@
         <v>3945</v>
       </c>
       <c r="D186">
-        <v>9990</v>
+        <v>1050</v>
       </c>
       <c r="E186">
         <v>11.8871</v>
@@ -9829,7 +9831,7 @@
       </c>
       <c r="G186" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 125</v>
       </c>
       <c r="H186" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9851,7 +9853,7 @@
         <v>3949</v>
       </c>
       <c r="D187">
-        <v>9990</v>
+        <v>1060</v>
       </c>
       <c r="E187">
         <v>11.8949</v>
@@ -9861,7 +9863,7 @@
       </c>
       <c r="G187" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 126</v>
       </c>
       <c r="H187" s="2" t="str">
         <f t="shared" si="7"/>
@@ -9883,7 +9885,7 @@
         <v>3953</v>
       </c>
       <c r="D188">
-        <v>9990</v>
+        <v>980</v>
       </c>
       <c r="E188">
         <v>11.8969</v>
@@ -9893,7 +9895,7 @@
       </c>
       <c r="G188" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 118</v>
       </c>
       <c r="H188" s="2" t="str">
         <f t="shared" si="7"/>
@@ -10043,7 +10045,7 @@
         <v>4026</v>
       </c>
       <c r="D193">
-        <v>9990</v>
+        <v>1070</v>
       </c>
       <c r="E193">
         <v>11.9903</v>
@@ -10053,7 +10055,7 @@
       </c>
       <c r="G193" t="str">
         <f t="shared" si="6"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 127</v>
       </c>
       <c r="H193" s="2" t="str">
         <f t="shared" si="7"/>
@@ -10107,7 +10109,7 @@
         <v>4030</v>
       </c>
       <c r="D195">
-        <v>9990</v>
+        <v>1060</v>
       </c>
       <c r="E195">
         <v>12.006600000000001</v>
@@ -10117,7 +10119,7 @@
       </c>
       <c r="G195" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 126</v>
       </c>
       <c r="H195" s="2" t="str">
         <f t="shared" si="10"/>
@@ -10171,7 +10173,7 @@
         <v>4038</v>
       </c>
       <c r="D197">
-        <v>9990</v>
+        <v>1030</v>
       </c>
       <c r="E197">
         <v>12.0314</v>
@@ -10181,7 +10183,7 @@
       </c>
       <c r="G197" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 123</v>
       </c>
       <c r="H197" s="2" t="str">
         <f t="shared" si="10"/>
@@ -10203,7 +10205,7 @@
         <v>4041</v>
       </c>
       <c r="D198">
-        <v>9990</v>
+        <v>1110</v>
       </c>
       <c r="E198">
         <v>12.0367</v>
@@ -10213,7 +10215,7 @@
       </c>
       <c r="G198" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 131</v>
       </c>
       <c r="H198" s="2" t="str">
         <f t="shared" si="10"/>
@@ -10299,7 +10301,7 @@
         <v>4088</v>
       </c>
       <c r="D201">
-        <v>9990</v>
+        <v>1030</v>
       </c>
       <c r="E201">
         <v>12.0928</v>
@@ -10309,7 +10311,7 @@
       </c>
       <c r="G201" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 123</v>
       </c>
       <c r="H201" s="2" t="str">
         <f t="shared" si="10"/>
@@ -10331,7 +10333,7 @@
         <v>4102</v>
       </c>
       <c r="D202">
-        <v>9990</v>
+        <v>1130</v>
       </c>
       <c r="E202">
         <v>12.106400000000001</v>
@@ -10341,7 +10343,7 @@
       </c>
       <c r="G202" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 133</v>
       </c>
       <c r="H202" s="2" t="str">
         <f t="shared" si="10"/>
@@ -10523,7 +10525,7 @@
         <v>4179</v>
       </c>
       <c r="D208">
-        <v>9990</v>
+        <v>1090</v>
       </c>
       <c r="E208">
         <v>12.214499999999999</v>
@@ -10533,7 +10535,7 @@
       </c>
       <c r="G208" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 129</v>
       </c>
       <c r="H208" s="2" t="str">
         <f t="shared" si="10"/>
@@ -10651,7 +10653,7 @@
         <v>4245</v>
       </c>
       <c r="D212">
-        <v>9990</v>
+        <v>1140</v>
       </c>
       <c r="E212">
         <v>12.2935</v>
@@ -10661,7 +10663,7 @@
       </c>
       <c r="G212" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 134</v>
       </c>
       <c r="H212" s="2" t="str">
         <f t="shared" si="10"/>
@@ -10683,7 +10685,7 @@
         <v>4251</v>
       </c>
       <c r="D213">
-        <v>9990</v>
+        <v>1060</v>
       </c>
       <c r="E213">
         <v>12.302300000000001</v>
@@ -10693,7 +10695,7 @@
       </c>
       <c r="G213" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 126</v>
       </c>
       <c r="H213" s="2" t="str">
         <f t="shared" si="10"/>
@@ -10779,7 +10781,7 @@
         <v>4273</v>
       </c>
       <c r="D216">
-        <v>9990</v>
+        <v>1170</v>
       </c>
       <c r="E216">
         <v>12.3322</v>
@@ -10789,7 +10791,7 @@
       </c>
       <c r="G216" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 137</v>
       </c>
       <c r="H216" s="2" t="str">
         <f t="shared" si="10"/>
@@ -10875,7 +10877,7 @@
         <v>4281</v>
       </c>
       <c r="D219">
-        <v>9990</v>
+        <v>1140</v>
       </c>
       <c r="E219">
         <v>12.3393</v>
@@ -10885,7 +10887,7 @@
       </c>
       <c r="G219" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 134</v>
       </c>
       <c r="H219" s="2" t="str">
         <f t="shared" si="10"/>
@@ -10907,7 +10909,7 @@
         <v>4293</v>
       </c>
       <c r="D220">
-        <v>9990</v>
+        <v>1030</v>
       </c>
       <c r="E220">
         <v>12.3536</v>
@@ -10917,7 +10919,7 @@
       </c>
       <c r="G220" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 123</v>
       </c>
       <c r="H220" s="2" t="str">
         <f t="shared" si="10"/>
@@ -11003,7 +11005,7 @@
         <v>4346</v>
       </c>
       <c r="D223">
-        <v>9990</v>
+        <v>1130</v>
       </c>
       <c r="E223">
         <v>12.3911</v>
@@ -11013,7 +11015,7 @@
       </c>
       <c r="G223" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 133</v>
       </c>
       <c r="H223" s="2" t="str">
         <f t="shared" si="10"/>
@@ -11099,7 +11101,7 @@
         <v>4365</v>
       </c>
       <c r="D226">
-        <v>9990</v>
+        <v>960</v>
       </c>
       <c r="E226">
         <v>12.4079</v>
@@ -11109,7 +11111,7 @@
       </c>
       <c r="G226" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 116</v>
       </c>
       <c r="H226" s="2" t="str">
         <f t="shared" si="10"/>
@@ -11163,7 +11165,7 @@
         <v>4394</v>
       </c>
       <c r="D228">
-        <v>9990</v>
+        <v>1090</v>
       </c>
       <c r="E228">
         <v>12.4321</v>
@@ -11173,7 +11175,7 @@
       </c>
       <c r="G228" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 129</v>
       </c>
       <c r="H228" s="2" t="str">
         <f t="shared" si="10"/>
@@ -11259,7 +11261,7 @@
         <v>4429</v>
       </c>
       <c r="D231">
-        <v>9990</v>
+        <v>1020</v>
       </c>
       <c r="E231">
         <v>12.4574</v>
@@ -11269,7 +11271,7 @@
       </c>
       <c r="G231" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 122</v>
       </c>
       <c r="H231" s="2" t="str">
         <f t="shared" si="10"/>
@@ -11355,7 +11357,7 @@
         <v>4442</v>
       </c>
       <c r="D234">
-        <v>9990</v>
+        <v>1040</v>
       </c>
       <c r="E234">
         <v>12.467700000000001</v>
@@ -11365,7 +11367,7 @@
       </c>
       <c r="G234" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 124</v>
       </c>
       <c r="H234" s="2" t="str">
         <f t="shared" si="10"/>
@@ -11387,7 +11389,7 @@
         <v>4448</v>
       </c>
       <c r="D235">
-        <v>9990</v>
+        <v>1120</v>
       </c>
       <c r="E235">
         <v>12.471</v>
@@ -11397,7 +11399,7 @@
       </c>
       <c r="G235" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 132</v>
       </c>
       <c r="H235" s="2" t="str">
         <f t="shared" si="10"/>
@@ -11483,7 +11485,7 @@
         <v>4459</v>
       </c>
       <c r="D238">
-        <v>9990</v>
+        <v>1040</v>
       </c>
       <c r="E238">
         <v>12.4833</v>
@@ -11493,7 +11495,7 @@
       </c>
       <c r="G238" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 124</v>
       </c>
       <c r="H238" s="2" t="str">
         <f t="shared" si="10"/>
@@ -11707,7 +11709,7 @@
         <v>4526</v>
       </c>
       <c r="D245">
-        <v>9990</v>
+        <v>960</v>
       </c>
       <c r="E245">
         <v>12.567500000000001</v>
@@ -11717,7 +11719,7 @@
       </c>
       <c r="G245" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 116</v>
       </c>
       <c r="H245" s="2" t="str">
         <f t="shared" si="10"/>
@@ -11739,7 +11741,7 @@
         <v>4527</v>
       </c>
       <c r="D246">
-        <v>9990</v>
+        <v>1050</v>
       </c>
       <c r="E246">
         <v>12.569000000000001</v>
@@ -11749,7 +11751,7 @@
       </c>
       <c r="G246" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 125</v>
       </c>
       <c r="H246" s="2" t="str">
         <f t="shared" si="10"/>
@@ -11771,7 +11773,7 @@
         <v>4535</v>
       </c>
       <c r="D247">
-        <v>9990</v>
+        <v>980</v>
       </c>
       <c r="E247">
         <v>12.5723</v>
@@ -11781,7 +11783,7 @@
       </c>
       <c r="G247" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 118</v>
       </c>
       <c r="H247" s="2" t="str">
         <f t="shared" si="10"/>
@@ -11995,7 +11997,7 @@
         <v>4570</v>
       </c>
       <c r="D254">
-        <v>9990</v>
+        <v>1080</v>
       </c>
       <c r="E254">
         <v>12.614800000000001</v>
@@ -12005,7 +12007,7 @@
       </c>
       <c r="G254" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 128</v>
       </c>
       <c r="H254" s="2" t="str">
         <f t="shared" si="10"/>
@@ -12059,7 +12061,7 @@
         <v>4596</v>
       </c>
       <c r="D256">
-        <v>9990</v>
+        <v>1050</v>
       </c>
       <c r="E256">
         <v>12.6655</v>
@@ -12069,7 +12071,7 @@
       </c>
       <c r="G256" t="str">
         <f t="shared" si="9"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 125</v>
       </c>
       <c r="H256" s="2" t="str">
         <f t="shared" si="10"/>
@@ -12187,7 +12189,7 @@
         <v>4643</v>
       </c>
       <c r="D260">
-        <v>9990</v>
+        <v>1080</v>
       </c>
       <c r="E260">
         <v>12.722300000000001</v>
@@ -12197,7 +12199,7 @@
       </c>
       <c r="G260" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 128</v>
       </c>
       <c r="H260" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12219,7 +12221,7 @@
         <v>4654</v>
       </c>
       <c r="D261">
-        <v>9990</v>
+        <v>1040</v>
       </c>
       <c r="E261">
         <v>12.7324</v>
@@ -12229,7 +12231,7 @@
       </c>
       <c r="G261" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 124</v>
       </c>
       <c r="H261" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12251,7 +12253,7 @@
         <v>4656</v>
       </c>
       <c r="D262">
-        <v>9990</v>
+        <v>1010</v>
       </c>
       <c r="E262">
         <v>12.732699999999999</v>
@@ -12261,7 +12263,7 @@
       </c>
       <c r="G262" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 121</v>
       </c>
       <c r="H262" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12283,7 +12285,7 @@
         <v>4660</v>
       </c>
       <c r="D263">
-        <v>9990</v>
+        <v>1120</v>
       </c>
       <c r="E263">
         <v>12.7422</v>
@@ -12293,7 +12295,7 @@
       </c>
       <c r="G263" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 132</v>
       </c>
       <c r="H263" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12315,7 +12317,7 @@
         <v>4666</v>
       </c>
       <c r="D264">
-        <v>9990</v>
+        <v>1080</v>
       </c>
       <c r="E264">
         <v>12.7524</v>
@@ -12325,7 +12327,7 @@
       </c>
       <c r="G264" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 128</v>
       </c>
       <c r="H264" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12347,7 +12349,7 @@
         <v>4689</v>
       </c>
       <c r="D265">
-        <v>9990</v>
+        <v>1070</v>
       </c>
       <c r="E265">
         <v>12.795999999999999</v>
@@ -12357,7 +12359,7 @@
       </c>
       <c r="G265" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 127</v>
       </c>
       <c r="H265" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12379,7 +12381,7 @@
         <v>4697</v>
       </c>
       <c r="D266">
-        <v>9990</v>
+        <v>920</v>
       </c>
       <c r="E266">
         <v>12.81</v>
@@ -12389,7 +12391,7 @@
       </c>
       <c r="G266" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 112</v>
       </c>
       <c r="H266" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12443,7 +12445,7 @@
         <v>4699</v>
       </c>
       <c r="D268">
-        <v>9990</v>
+        <v>960</v>
       </c>
       <c r="E268">
         <v>12.817299999999999</v>
@@ -12453,7 +12455,7 @@
       </c>
       <c r="G268" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 116</v>
       </c>
       <c r="H268" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12539,7 +12541,7 @@
         <v>4754</v>
       </c>
       <c r="D271">
-        <v>9990</v>
+        <v>1050</v>
       </c>
       <c r="E271">
         <v>12.871499999999999</v>
@@ -12549,7 +12551,7 @@
       </c>
       <c r="G271" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 125</v>
       </c>
       <c r="H271" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12571,7 +12573,7 @@
         <v>4762</v>
       </c>
       <c r="D272">
-        <v>9990</v>
+        <v>1010</v>
       </c>
       <c r="E272">
         <v>12.882199999999999</v>
@@ -12581,7 +12583,7 @@
       </c>
       <c r="G272" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 121</v>
       </c>
       <c r="H272" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12603,7 +12605,7 @@
         <v>4781</v>
       </c>
       <c r="D273">
-        <v>9990</v>
+        <v>1110</v>
       </c>
       <c r="E273">
         <v>12.906599999999999</v>
@@ -12613,7 +12615,7 @@
       </c>
       <c r="G273" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 131</v>
       </c>
       <c r="H273" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12635,7 +12637,7 @@
         <v>4800</v>
       </c>
       <c r="D274">
-        <v>9990</v>
+        <v>1160</v>
       </c>
       <c r="E274">
         <v>12.910500000000001</v>
@@ -12645,7 +12647,7 @@
       </c>
       <c r="G274" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 136</v>
       </c>
       <c r="H274" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12699,7 +12701,7 @@
         <v>4856</v>
       </c>
       <c r="D276">
-        <v>9990</v>
+        <v>1060</v>
       </c>
       <c r="E276">
         <v>12.9892</v>
@@ -12709,7 +12711,7 @@
       </c>
       <c r="G276" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 126</v>
       </c>
       <c r="H276" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12731,7 +12733,7 @@
         <v>4866</v>
       </c>
       <c r="D277">
-        <v>9990</v>
+        <v>1110</v>
       </c>
       <c r="E277">
         <v>12.9909</v>
@@ -12741,7 +12743,7 @@
       </c>
       <c r="G277" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 131</v>
       </c>
       <c r="H277" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12763,7 +12765,7 @@
         <v>4900</v>
       </c>
       <c r="D278">
-        <v>9990</v>
+        <v>1130</v>
       </c>
       <c r="E278">
         <v>13.010899999999999</v>
@@ -12773,7 +12775,7 @@
       </c>
       <c r="G278" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 133</v>
       </c>
       <c r="H278" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12795,7 +12797,7 @@
         <v>4958</v>
       </c>
       <c r="D279">
-        <v>9990</v>
+        <v>1070</v>
       </c>
       <c r="E279">
         <v>13.0969</v>
@@ -12805,7 +12807,7 @@
       </c>
       <c r="G279" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 127</v>
       </c>
       <c r="H279" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12827,7 +12829,7 @@
         <v>4995</v>
       </c>
       <c r="D280">
-        <v>9990</v>
+        <v>1120</v>
       </c>
       <c r="E280">
         <v>13.161300000000001</v>
@@ -12837,7 +12839,7 @@
       </c>
       <c r="G280" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 132</v>
       </c>
       <c r="H280" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12923,7 +12925,7 @@
         <v>5054</v>
       </c>
       <c r="D283">
-        <v>9990</v>
+        <v>1090</v>
       </c>
       <c r="E283">
         <v>13.2829</v>
@@ -12933,7 +12935,7 @@
       </c>
       <c r="G283" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 129</v>
       </c>
       <c r="H283" s="2" t="str">
         <f t="shared" si="13"/>
@@ -12987,7 +12989,7 @@
         <v>5248</v>
       </c>
       <c r="D285">
-        <v>9990</v>
+        <v>1010</v>
       </c>
       <c r="E285">
         <v>13.6256</v>
@@ -12997,7 +12999,7 @@
       </c>
       <c r="G285" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 121</v>
       </c>
       <c r="H285" s="2" t="str">
         <f t="shared" si="13"/>
@@ -13051,7 +13053,7 @@
         <v>5322</v>
       </c>
       <c r="D287">
-        <v>9990</v>
+        <v>1010</v>
       </c>
       <c r="E287">
         <v>13.8209</v>
@@ -13061,7 +13063,7 @@
       </c>
       <c r="G287" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 121</v>
       </c>
       <c r="H287" s="2" t="str">
         <f t="shared" si="13"/>
@@ -13147,7 +13149,7 @@
         <v>5473</v>
       </c>
       <c r="D290">
-        <v>9990</v>
+        <v>1140</v>
       </c>
       <c r="E290">
         <v>14.0787</v>
@@ -13157,7 +13159,7 @@
       </c>
       <c r="G290" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 134</v>
       </c>
       <c r="H290" s="2" t="str">
         <f t="shared" si="13"/>
@@ -13211,7 +13213,7 @@
         <v>5557</v>
       </c>
       <c r="D292">
-        <v>9990</v>
+        <v>1090</v>
       </c>
       <c r="E292">
         <v>14.3071</v>
@@ -13221,7 +13223,7 @@
       </c>
       <c r="G292" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 129</v>
       </c>
       <c r="H292" s="2" t="str">
         <f t="shared" si="13"/>
@@ -13371,7 +13373,7 @@
         <v>5676</v>
       </c>
       <c r="D297">
-        <v>9990</v>
+        <v>1110</v>
       </c>
       <c r="E297">
         <v>14.5463</v>
@@ -13381,7 +13383,7 @@
       </c>
       <c r="G297" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 131</v>
       </c>
       <c r="H297" s="2" t="str">
         <f t="shared" si="13"/>
@@ -13403,7 +13405,7 @@
         <v>5689</v>
       </c>
       <c r="D298">
-        <v>9990</v>
+        <v>1190</v>
       </c>
       <c r="E298">
         <v>14.5916</v>
@@ -13413,7 +13415,7 @@
       </c>
       <c r="G298" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 139</v>
       </c>
       <c r="H298" s="2" t="str">
         <f t="shared" si="13"/>
@@ -13467,7 +13469,7 @@
         <v>5746</v>
       </c>
       <c r="D300">
-        <v>9990</v>
+        <v>1050</v>
       </c>
       <c r="E300">
         <v>14.748900000000001</v>
@@ -13477,7 +13479,7 @@
       </c>
       <c r="G300" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 125</v>
       </c>
       <c r="H300" s="2" t="str">
         <f t="shared" si="13"/>
@@ -13499,7 +13501,7 @@
         <v>5846</v>
       </c>
       <c r="D301">
-        <v>9990</v>
+        <v>1010</v>
       </c>
       <c r="E301">
         <v>15.1081</v>
@@ -13509,7 +13511,7 @@
       </c>
       <c r="G301" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 121</v>
       </c>
       <c r="H301" s="2" t="str">
         <f t="shared" si="13"/>
@@ -13595,7 +13597,7 @@
         <v>5982</v>
       </c>
       <c r="D304">
-        <v>9990</v>
+        <v>1100</v>
       </c>
       <c r="E304">
         <v>15.644399999999999</v>
@@ -13605,7 +13607,7 @@
       </c>
       <c r="G304" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 130</v>
       </c>
       <c r="H304" s="2" t="str">
         <f t="shared" si="13"/>
@@ -13627,7 +13629,7 @@
         <v>6118</v>
       </c>
       <c r="D305">
-        <v>9990</v>
+        <v>1170</v>
       </c>
       <c r="E305">
         <v>16.363499999999998</v>
@@ -13637,7 +13639,7 @@
       </c>
       <c r="G305" t="str">
         <f t="shared" si="12"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 137</v>
       </c>
       <c r="H305" s="2" t="str">
         <f t="shared" si="13"/>
@@ -14171,7 +14173,7 @@
         <v>6426</v>
       </c>
       <c r="D322">
-        <v>9990</v>
+        <v>1090</v>
       </c>
       <c r="E322">
         <v>17.7485</v>
@@ -14181,7 +14183,7 @@
       </c>
       <c r="G322" t="str">
         <f t="shared" ref="G322:G385" si="15">RIGHT("              "&amp;TRUNC((D322+200)/10),4)</f>
-        <v>1019</v>
+        <v xml:space="preserve"> 129</v>
       </c>
       <c r="H322" s="2" t="str">
         <f t="shared" ref="H322:H385" si="16">RIGHT("              " &amp;TRUNC(E322*65536 / 24),6)</f>
@@ -14331,7 +14333,7 @@
         <v>6517</v>
       </c>
       <c r="D327">
-        <v>9990</v>
+        <v>1010</v>
       </c>
       <c r="E327">
         <v>18.0307</v>
@@ -14341,7 +14343,7 @@
       </c>
       <c r="G327" t="str">
         <f t="shared" si="15"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 121</v>
       </c>
       <c r="H327" s="2" t="str">
         <f t="shared" si="16"/>
@@ -14459,7 +14461,7 @@
         <v>6540</v>
       </c>
       <c r="D331">
-        <v>9990</v>
+        <v>1460</v>
       </c>
       <c r="E331">
         <v>18.1022</v>
@@ -14469,7 +14471,7 @@
       </c>
       <c r="G331" t="str">
         <f t="shared" si="15"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 166</v>
       </c>
       <c r="H331" s="2" t="str">
         <f t="shared" si="16"/>
@@ -14555,7 +14557,7 @@
         <v>6553</v>
       </c>
       <c r="D334">
-        <v>9990</v>
+        <v>830</v>
       </c>
       <c r="E334">
         <v>18.154900000000001</v>
@@ -14565,7 +14567,7 @@
       </c>
       <c r="G334" t="str">
         <f t="shared" si="15"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 103</v>
       </c>
       <c r="H334" s="2" t="str">
         <f t="shared" si="16"/>
@@ -14683,7 +14685,7 @@
         <v>6624</v>
       </c>
       <c r="D338">
-        <v>9990</v>
+        <v>760</v>
       </c>
       <c r="E338">
         <v>18.394600000000001</v>
@@ -14693,7 +14695,7 @@
       </c>
       <c r="G338" t="str">
         <f t="shared" si="15"/>
-        <v>1019</v>
+        <v xml:space="preserve">  96</v>
       </c>
       <c r="H338" s="2" t="str">
         <f t="shared" si="16"/>
@@ -15451,7 +15453,7 @@
         <v>6946</v>
       </c>
       <c r="D362">
-        <v>9990</v>
+        <v>900</v>
       </c>
       <c r="E362">
         <v>20.581199999999999</v>
@@ -15461,7 +15463,7 @@
       </c>
       <c r="G362" t="str">
         <f t="shared" si="15"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 110</v>
       </c>
       <c r="H362" s="2" t="str">
         <f t="shared" si="16"/>
@@ -15483,7 +15485,7 @@
         <v>7000</v>
       </c>
       <c r="D363">
-        <v>9990</v>
+        <v>500</v>
       </c>
       <c r="E363">
         <v>20.988099999999999</v>
@@ -15493,7 +15495,7 @@
       </c>
       <c r="G363" t="str">
         <f t="shared" si="15"/>
-        <v>1019</v>
+        <v xml:space="preserve">  70</v>
       </c>
       <c r="H363" s="2" t="str">
         <f t="shared" si="16"/>
@@ -15963,7 +15965,7 @@
         <v>7448</v>
       </c>
       <c r="D378">
-        <v>9990</v>
+        <v>1140</v>
       </c>
       <c r="E378">
         <v>23.001000000000001</v>
@@ -15973,7 +15975,7 @@
       </c>
       <c r="G378" t="str">
         <f t="shared" si="15"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 134</v>
       </c>
       <c r="H378" s="2" t="str">
         <f t="shared" si="16"/>
@@ -16059,7 +16061,7 @@
         <v>7606</v>
       </c>
       <c r="D381">
-        <v>9990</v>
+        <v>1080</v>
       </c>
       <c r="E381">
         <v>23.318000000000001</v>
@@ -16069,7 +16071,7 @@
       </c>
       <c r="G381" t="str">
         <f t="shared" si="15"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 128</v>
       </c>
       <c r="H381" s="2" t="str">
         <f t="shared" si="16"/>
@@ -16155,7 +16157,7 @@
         <v>7723</v>
       </c>
       <c r="D384">
-        <v>9990</v>
+        <v>1120</v>
       </c>
       <c r="E384">
         <v>23.6492</v>
@@ -16165,7 +16167,7 @@
       </c>
       <c r="G384" t="str">
         <f t="shared" si="15"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 132</v>
       </c>
       <c r="H384" s="2" t="str">
         <f t="shared" si="16"/>
@@ -16187,7 +16189,7 @@
         <v>7727</v>
       </c>
       <c r="D385">
-        <v>9990</v>
+        <v>1060</v>
       </c>
       <c r="E385">
         <v>23.664899999999999</v>
@@ -16197,7 +16199,7 @@
       </c>
       <c r="G385" t="str">
         <f t="shared" si="15"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 126</v>
       </c>
       <c r="H385" s="2" t="str">
         <f t="shared" si="16"/>
@@ -16283,7 +16285,7 @@
         <v>7814</v>
       </c>
       <c r="D388">
-        <v>9990</v>
+        <v>1080</v>
       </c>
       <c r="E388">
         <v>5.4100000000000002E-2</v>
@@ -16293,7 +16295,7 @@
       </c>
       <c r="G388" t="str">
         <f t="shared" si="18"/>
-        <v>1019</v>
+        <v xml:space="preserve"> 128</v>
       </c>
       <c r="H388" s="2" t="str">
         <f t="shared" si="19"/>

</xml_diff>